<commit_message>
survey code updated from 1 to right ones
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_9.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_9.xlsx
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">template!$A$1:$V$73</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">template!$A$1:$V$73</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">template!$A$1:$V$73</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$V$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1002,23 +1003,25 @@
   </sheetPr>
   <dimension ref="1:73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S45" activeCellId="0" sqref="S45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.9183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="69.0816326530612"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="101.244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.2397959183674"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="65.1479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="68.3061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="100.163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="1" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9585,7 +9588,7 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -9601,7 +9604,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="n">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>61</v>
@@ -10705,7 +10708,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>66</v>
       </c>
@@ -10721,7 +10724,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>75</v>
@@ -11769,7 +11772,7 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
         <v>66</v>
       </c>
@@ -11785,7 +11788,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11" t="n">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>80</v>
@@ -18133,7 +18136,7 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>66</v>
       </c>
@@ -21337,7 +21340,7 @@
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
         <v>66</v>
       </c>
@@ -22537,7 +22540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
         <v>113</v>
       </c>
@@ -22553,7 +22556,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16" t="n">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>80</v>
@@ -27841,7 +27844,7 @@
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
         <v>113</v>
       </c>
@@ -36337,7 +36340,7 @@
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
@@ -37405,7 +37408,7 @@
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -37421,7 +37424,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8" t="n">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>61</v>
@@ -43777,7 +43780,7 @@
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>123</v>
       </c>
@@ -44845,7 +44848,7 @@
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>123</v>
       </c>
@@ -44861,7 +44864,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8" t="n">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>61</v>
@@ -48025,7 +48028,7 @@
       <c r="AMI48" s="0"/>
       <c r="AMJ48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="23" t="s">
         <v>124</v>
       </c>
@@ -54529,11 +54532,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:V73">
-    <filterColumn colId="18">
-      <filters>
-        <filter val="Exhibicion Especial, Big Bet"/>
-        <filter val="POP Interior, POP Exterior"/>
-      </filters>
+    <filterColumn colId="21">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Survey"/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -54560,7 +54562,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54687,7 +54689,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>